<commit_message>
Koncano delo na nalogi (upam)
</commit_message>
<xml_diff>
--- a/plan/razredni diagram.xlsx
+++ b/plan/razredni diagram.xlsx
@@ -32,12 +32,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>+ String preberiEhrIdZaVitalneZnake</t>
-  </si>
-  <si>
-    <t>+ String meritveVitalnihZnakovEHRid</t>
-  </si>
-  <si>
     <t>+ generiraj()</t>
   </si>
   <si>
@@ -53,18 +47,6 @@
     <t>vnos</t>
   </si>
   <si>
-    <t>+ String meritevEHRId</t>
-  </si>
-  <si>
-    <t>+ Int meritevVisina</t>
-  </si>
-  <si>
-    <t>+ String meritevDatum</t>
-  </si>
-  <si>
-    <t>+ Int meritevTeza</t>
-  </si>
-  <si>
     <t>+ vnosMeritev()</t>
   </si>
   <si>
@@ -74,69 +56,15 @@
     <t>koda</t>
   </si>
   <si>
-    <t>- String baseUrl</t>
-  </si>
-  <si>
-    <t>- String queryUrl</t>
-  </si>
-  <si>
-    <t>- String username</t>
-  </si>
-  <si>
-    <t>- String password</t>
-  </si>
-  <si>
-    <t>- Int_array items</t>
-  </si>
-  <si>
-    <t>- Int_array visina</t>
-  </si>
-  <si>
-    <t>- Int_array teza</t>
-  </si>
-  <si>
-    <t>- Int_array dat</t>
-  </si>
-  <si>
-    <t>- Int_array gBMI</t>
-  </si>
-  <si>
-    <t>- Int manj</t>
-  </si>
-  <si>
-    <t>- Int vec</t>
-  </si>
-  <si>
-    <t>- Float scale</t>
-  </si>
-  <si>
     <t># getSessionId()</t>
   </si>
   <si>
-    <t>- generirajPodatke(Int stPacienta)</t>
-  </si>
-  <si>
-    <t>- String kreirajNovEhr(String ime, String priimek, String datumRojstva)</t>
-  </si>
-  <si>
     <t>- pridobiStatisticnePodatke()</t>
   </si>
   <si>
-    <t>- log(String text)</t>
-  </si>
-  <si>
     <t>- grafFunkcija()</t>
   </si>
   <si>
-    <t>- Int width(Int margin)</t>
-  </si>
-  <si>
-    <t>- Int height(Int margin)</t>
-  </si>
-  <si>
-    <t>- sortFunction(Int a, Int b)</t>
-  </si>
-  <si>
     <t>- generateData()</t>
   </si>
   <si>
@@ -152,16 +80,88 @@
     <t># https://rest.ehrscape.com/rest/v1/</t>
   </si>
   <si>
-    <t>+ String session(String username, String password)</t>
-  </si>
-  <si>
-    <t>+ JSON_object demographics/EHR/EHRid/parity (String sessionID, String EHRid)</t>
-  </si>
-  <si>
-    <t>+ JSON_array view/EHRid/weight(String sessionID, String EHRid)</t>
-  </si>
-  <si>
-    <t>+ JSON_array view/EHRid/height(String sessionID, String EHRid)</t>
+    <t xml:space="preserve">- baseUrl : String </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- queryUrl : String </t>
+  </si>
+  <si>
+    <t>- username : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- password : String </t>
+  </si>
+  <si>
+    <t>- items : Int_array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- visina : Int_array </t>
+  </si>
+  <si>
+    <t>- teza : Int_array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- dat : Int_array </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- gBMI : Int_array </t>
+  </si>
+  <si>
+    <t>- manj : Int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- vec : Int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- scale : Float </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ preberiEhrIdZaVitalneZnake : String </t>
+  </si>
+  <si>
+    <t>+ meritveVitalnihZnakovEHRid : String</t>
+  </si>
+  <si>
+    <t>+ meritevEHRId : String</t>
+  </si>
+  <si>
+    <t>+ meritevVisina : Int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ meritevTeza : Int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ meritevDatum : String </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- kreirajNovEhr(ime : String, priimek : String, datumRojstva : String) : String </t>
+  </si>
+  <si>
+    <t>- Int width(margin : Int)</t>
+  </si>
+  <si>
+    <t>- Int height(margin : Int)</t>
+  </si>
+  <si>
+    <t>- sortFunction(a : Int, Int b : Int)</t>
+  </si>
+  <si>
+    <t>- generirajPodatke(stPacienta : Int)</t>
+  </si>
+  <si>
+    <t>- log(text : String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ session(username : String, password : String) : String </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ demographics/EHR/EHRid/parity (sessionID : String, EHRid : String) :  JSON_object </t>
+  </si>
+  <si>
+    <t>+ view/EHRid/weight(sessionID : String, EHRid : String) : JSON_array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ view/EHRid/height(sessionID : String, EHRid : String) : JSON_array </t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,9 +558,9 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="34.5703125" style="1" customWidth="1"/>
     <col min="4" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="63.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="67" style="1" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="71.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="77" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -579,23 +579,23 @@
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>42</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>43</v>
@@ -614,10 +614,10 @@
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>44</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>45</v>
@@ -636,27 +636,27 @@
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G11" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G12" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G14" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G15" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
@@ -664,135 +664,135 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G23" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G24" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G25" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G26" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G27" s="5" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G28" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G29" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G30" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G31" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G32" s="5" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" s="5" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G38" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>